<commit_message>
Add test for date bug in a style format
</commit_message>
<xml_diff>
--- a/tests/testthat/date-bug.xlsx
+++ b/tests/testthat/date-bug.xlsx
@@ -17,7 +17,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,14 +50,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="date" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -350,9 +360,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -364,8 +376,14 @@
         <v>60.9</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>60.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>